<commit_message>
Rename and refactor files for better structure
Moved `permutation.ipynb` and `instruments_graph.ipynb` to an `old` directory to clean the workspace. Refactored `permutation.ipynb` into a script-based format for improved readability and maintainability.
</commit_message>
<xml_diff>
--- a/TOOLS/generate_decision_tree/Instrument_tree.xlsx
+++ b/TOOLS/generate_decision_tree/Instrument_tree.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Documents\PYTHON\FragHub\TOOLS\generate_decision_tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Axel\PYTHON\FragHub\TOOLS\generate_decision_tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB114A39-127D-4694-880B-55CB7BA12948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADC7BC6-7621-4A5D-9746-89363DB9B896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB SCIEX" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="325">
   <si>
     <t>MARQUES</t>
   </si>
@@ -1000,13 +1000,16 @@
   </si>
   <si>
     <t>CE</t>
+  </si>
+  <si>
+    <t>IE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,6 +1021,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1058,11 +1074,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3568,10 +3586,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3582,6 +3600,7 @@
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4224,7 +4243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>127</v>
       </c>
@@ -4244,18 +4263,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>127</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
@@ -4264,18 +4283,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>127</v>
       </c>
       <c r="B35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>166</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
         <v>31</v>
@@ -4284,7 +4303,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -4295,7 +4314,7 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
         <v>31</v>
@@ -4304,12 +4323,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>127</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -4324,7 +4343,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -4338,18 +4357,18 @@
         <v>166</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -4358,61 +4377,61 @@
         <v>166</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C40" t="s">
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s">
         <v>31</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D41" t="s">
         <v>27</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
+        <v>167</v>
       </c>
       <c r="F41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -4424,12 +4443,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
         <v>26</v>
@@ -4444,12 +4463,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
         <v>26</v>
@@ -4464,45 +4483,150 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E45" t="s">
-        <v>167</v>
+        <v>50</v>
       </c>
       <c r="F45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B46" t="s">
-        <v>163</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B46" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F46" t="s">
-        <v>34</v>
-      </c>
+      <c r="F48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4513,7 +4637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>

</xml_diff>